<commit_message>
Standardize the DB tables and the dummy values
</commit_message>
<xml_diff>
--- a/sample_excel.xlsx
+++ b/sample_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\ttsh-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BCD4BF-7FD1-48D9-AC3D-D544E9F45F46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD5508B-B542-41C2-94B8-4955F4A212E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="5" r:id="rId1"/>
@@ -19,9 +19,6 @@
     <sheet name="Priority Leave" sheetId="3" r:id="rId4"/>
     <sheet name="Public Holiday" sheetId="4" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="212">
   <si>
     <t>Email</t>
   </si>
@@ -446,9 +443,6 @@
     <t>AR</t>
   </si>
   <si>
-    <t>AS</t>
-  </si>
-  <si>
     <t>AT</t>
   </si>
   <si>
@@ -677,19 +671,10 @@
     <t>P48</t>
   </si>
   <si>
-    <t>Clashing1</t>
-  </si>
-  <si>
-    <t>Clashing2</t>
-  </si>
-  <si>
     <t>NotClashing1</t>
   </si>
   <si>
-    <t>Clashing3</t>
-  </si>
-  <si>
-    <t>Clashing4</t>
+    <t>ASB</t>
   </si>
 </sst>
 </file>
@@ -824,428 +809,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Roster"/>
-      <sheetName val="Duties"/>
-      <sheetName val="Training"/>
-      <sheetName val="Priority Leave"/>
-      <sheetName val="Public Holiday"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>V</v>
-          </cell>
-          <cell r="B2">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>W</v>
-          </cell>
-          <cell r="B3">
-            <v>23</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>X</v>
-          </cell>
-          <cell r="B4">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Y</v>
-          </cell>
-          <cell r="B5">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Z</v>
-          </cell>
-          <cell r="B6">
-            <v>26</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>AA</v>
-          </cell>
-          <cell r="B7">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>AB</v>
-          </cell>
-          <cell r="B8">
-            <v>28</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>AC</v>
-          </cell>
-          <cell r="B9">
-            <v>29</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>AD</v>
-          </cell>
-          <cell r="B10">
-            <v>30</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>AE</v>
-          </cell>
-          <cell r="B11">
-            <v>31</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>AF</v>
-          </cell>
-          <cell r="B12">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>AG</v>
-          </cell>
-          <cell r="B13">
-            <v>33</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>AH</v>
-          </cell>
-          <cell r="B14">
-            <v>34</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>AI</v>
-          </cell>
-          <cell r="B15">
-            <v>35</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>AJ</v>
-          </cell>
-          <cell r="B16">
-            <v>36</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>AK</v>
-          </cell>
-          <cell r="B17">
-            <v>37</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>AL</v>
-          </cell>
-          <cell r="B18">
-            <v>38</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>AM</v>
-          </cell>
-          <cell r="B19">
-            <v>39</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>AN</v>
-          </cell>
-          <cell r="B20">
-            <v>40</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>AO</v>
-          </cell>
-          <cell r="B21">
-            <v>41</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>AP</v>
-          </cell>
-          <cell r="B22">
-            <v>42</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>AQ</v>
-          </cell>
-          <cell r="B23">
-            <v>43</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>AR</v>
-          </cell>
-          <cell r="B24">
-            <v>44</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>AS</v>
-          </cell>
-          <cell r="B25">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>AT</v>
-          </cell>
-          <cell r="B26">
-            <v>46</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>AV</v>
-          </cell>
-          <cell r="B27">
-            <v>47</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>AW</v>
-          </cell>
-          <cell r="B28">
-            <v>48</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>AX</v>
-          </cell>
-          <cell r="B29">
-            <v>49</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>AY</v>
-          </cell>
-          <cell r="B30">
-            <v>50</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>A</v>
-          </cell>
-          <cell r="B31">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>B</v>
-          </cell>
-          <cell r="B32">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="B33">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>D</v>
-          </cell>
-          <cell r="B34">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>E</v>
-          </cell>
-          <cell r="B35">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>F</v>
-          </cell>
-          <cell r="B36">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>G</v>
-          </cell>
-          <cell r="B37">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>H</v>
-          </cell>
-          <cell r="B38">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39" t="str">
-            <v>I</v>
-          </cell>
-          <cell r="B39">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40" t="str">
-            <v>J</v>
-          </cell>
-          <cell r="B40">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41" t="str">
-            <v>K</v>
-          </cell>
-          <cell r="B41">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42" t="str">
-            <v>L</v>
-          </cell>
-          <cell r="B42">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43" t="str">
-            <v>M</v>
-          </cell>
-          <cell r="B43">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="B44">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45" t="str">
-            <v>O</v>
-          </cell>
-          <cell r="B45">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46" t="str">
-            <v>P</v>
-          </cell>
-          <cell r="B46">
-            <v>16</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47" t="str">
-            <v>Q</v>
-          </cell>
-          <cell r="B47">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48" t="str">
-            <v>R</v>
-          </cell>
-          <cell r="B48">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49" t="str">
-            <v>S</v>
-          </cell>
-          <cell r="B49">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50" t="str">
-            <v>T</v>
-          </cell>
-          <cell r="B50">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51" t="str">
-            <v>U</v>
-          </cell>
-          <cell r="B51">
-            <v>21</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1513,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402572E3-A301-453A-BBD2-7FEA71DA364E}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1552,8 +1115,8 @@
       <c r="A2" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="12">
-        <v>22</v>
+      <c r="B2" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>103</v>
@@ -1575,8 +1138,8 @@
       <c r="A3" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="12">
-        <v>23</v>
+      <c r="B3" s="14" t="s">
+        <v>112</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>103</v>
@@ -1598,8 +1161,8 @@
       <c r="A4" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="12">
-        <v>24</v>
+      <c r="B4" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -1621,8 +1184,8 @@
       <c r="A5" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="12">
-        <v>25</v>
+      <c r="B5" s="14" t="s">
+        <v>104</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>103</v>
@@ -1644,8 +1207,8 @@
       <c r="A6" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="12">
-        <v>26</v>
+      <c r="B6" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>103</v>
@@ -1667,8 +1230,8 @@
       <c r="A7" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="12">
-        <v>27</v>
+      <c r="B7" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>103</v>
@@ -1690,8 +1253,8 @@
       <c r="A8" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="12">
-        <v>28</v>
+      <c r="B8" s="14" t="s">
+        <v>116</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>103</v>
@@ -1713,8 +1276,8 @@
       <c r="A9" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="12">
-        <v>29</v>
+      <c r="B9" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>103</v>
@@ -1736,8 +1299,8 @@
       <c r="A10" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="12">
-        <v>30</v>
+      <c r="B10" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>103</v>
@@ -1759,8 +1322,8 @@
       <c r="A11" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="12">
-        <v>31</v>
+      <c r="B11" s="14" t="s">
+        <v>119</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>120</v>
@@ -1782,8 +1345,8 @@
       <c r="A12" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="12">
-        <v>32</v>
+      <c r="B12" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>120</v>
@@ -1805,8 +1368,8 @@
       <c r="A13" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="12">
-        <v>33</v>
+      <c r="B13" s="14" t="s">
+        <v>122</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>120</v>
@@ -1828,8 +1391,8 @@
       <c r="A14" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="12">
-        <v>34</v>
+      <c r="B14" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>120</v>
@@ -1851,8 +1414,8 @@
       <c r="A15" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="12">
-        <v>35</v>
+      <c r="B15" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>120</v>
@@ -1874,8 +1437,8 @@
       <c r="A16" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B16" s="12">
-        <v>36</v>
+      <c r="B16" s="14" t="s">
+        <v>125</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>120</v>
@@ -1897,8 +1460,8 @@
       <c r="A17" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="12">
-        <v>37</v>
+      <c r="B17" s="14" t="s">
+        <v>126</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>120</v>
@@ -1920,17 +1483,17 @@
       <c r="A18" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="12">
-        <v>38</v>
+      <c r="B18" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D18" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>143</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>144</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>82</v>
@@ -1943,17 +1506,17 @@
       <c r="A19" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="12">
-        <v>39</v>
+      <c r="B19" s="14" t="s">
+        <v>128</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D19" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>145</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>146</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>78</v>
@@ -1966,17 +1529,17 @@
       <c r="A20" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="12">
-        <v>40</v>
+      <c r="B20" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D20" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>147</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>148</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>101</v>
@@ -1989,17 +1552,17 @@
       <c r="A21" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="B21" s="12">
-        <v>41</v>
+      <c r="B21" s="14" t="s">
+        <v>130</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D21" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>149</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>150</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>82</v>
@@ -2012,17 +1575,17 @@
       <c r="A22" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B22" s="12">
-        <v>42</v>
+      <c r="B22" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D22" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>151</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>152</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>102</v>
@@ -2035,17 +1598,17 @@
       <c r="A23" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B23" s="12">
-        <v>43</v>
+      <c r="B23" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D23" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>153</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>154</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>82</v>
@@ -2058,17 +1621,17 @@
       <c r="A24" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B24" s="12">
-        <v>44</v>
+      <c r="B24" s="14" t="s">
+        <v>133</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D24" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>155</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>156</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>78</v>
@@ -2079,19 +1642,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B25" s="12">
-        <v>45</v>
+        <v>211</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>211</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D25" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>157</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>101</v>
@@ -2102,19 +1665,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B26" s="12">
-        <v>46</v>
+        <v>134</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D26" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>160</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>82</v>
@@ -2125,19 +1688,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B27" s="12">
-        <v>47</v>
+        <v>135</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>135</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D27" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>161</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>102</v>
@@ -2148,19 +1711,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B28" s="12">
-        <v>48</v>
+        <v>136</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D28" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>163</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>164</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>82</v>
@@ -2171,19 +1734,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B29" s="12">
-        <v>49</v>
+        <v>137</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>137</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D29" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="13" t="s">
         <v>165</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>166</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>78</v>
@@ -2194,19 +1757,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B30" s="12">
-        <v>50</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>140</v>
-      </c>
       <c r="D30" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E30" s="13" t="s">
         <v>167</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>168</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>101</v>
@@ -2219,17 +1782,17 @@
       <c r="A31" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="12">
-        <v>1</v>
+      <c r="B31" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D31" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E31" s="13" t="s">
         <v>169</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>170</v>
       </c>
       <c r="F31" s="13" t="s">
         <v>82</v>
@@ -2242,17 +1805,17 @@
       <c r="A32" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="12">
-        <v>2</v>
+      <c r="B32" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D32" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>171</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>172</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>102</v>
@@ -2265,17 +1828,17 @@
       <c r="A33" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="12">
-        <v>3</v>
+      <c r="B33" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D33" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>173</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>174</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>82</v>
@@ -2288,17 +1851,17 @@
       <c r="A34" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="12">
-        <v>4</v>
+      <c r="B34" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D34" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="E34" s="13" t="s">
         <v>175</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>176</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>78</v>
@@ -2311,17 +1874,17 @@
       <c r="A35" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="12">
-        <v>5</v>
+      <c r="B35" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D35" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="13" t="s">
         <v>177</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>178</v>
       </c>
       <c r="F35" s="13" t="s">
         <v>101</v>
@@ -2334,17 +1897,17 @@
       <c r="A36" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="12">
-        <v>6</v>
+      <c r="B36" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D36" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E36" s="13" t="s">
         <v>179</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>180</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>82</v>
@@ -2357,17 +1920,17 @@
       <c r="A37" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="12">
-        <v>7</v>
+      <c r="B37" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D37" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>181</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>182</v>
       </c>
       <c r="F37" s="13" t="s">
         <v>102</v>
@@ -2380,17 +1943,17 @@
       <c r="A38" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="12">
-        <v>8</v>
+      <c r="B38" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D38" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="E38" s="12" t="s">
         <v>183</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>184</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>82</v>
@@ -2403,17 +1966,17 @@
       <c r="A39" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="12">
-        <v>9</v>
+      <c r="B39" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D39" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" s="13" t="s">
         <v>185</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>186</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>78</v>
@@ -2426,17 +1989,17 @@
       <c r="A40" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="12">
-        <v>10</v>
+      <c r="B40" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D40" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E40" s="13" t="s">
         <v>187</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>188</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>101</v>
@@ -2449,17 +2012,17 @@
       <c r="A41" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="12">
-        <v>11</v>
+      <c r="B41" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D41" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>189</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>190</v>
       </c>
       <c r="F41" s="13" t="s">
         <v>82</v>
@@ -2472,17 +2035,17 @@
       <c r="A42" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="12">
-        <v>12</v>
+      <c r="B42" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D42" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>191</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>192</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>102</v>
@@ -2495,17 +2058,17 @@
       <c r="A43" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="12">
-        <v>13</v>
+      <c r="B43" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D43" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="E43" s="12" t="s">
         <v>193</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>194</v>
       </c>
       <c r="F43" s="12" t="s">
         <v>82</v>
@@ -2518,17 +2081,17 @@
       <c r="A44" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="12">
-        <v>14</v>
+      <c r="B44" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D44" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E44" s="13" t="s">
         <v>195</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>196</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>78</v>
@@ -2541,17 +2104,17 @@
       <c r="A45" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="12">
-        <v>15</v>
+      <c r="B45" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D45" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="E45" s="13" t="s">
         <v>197</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>101</v>
@@ -2564,17 +2127,17 @@
       <c r="A46" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="12">
-        <v>16</v>
+      <c r="B46" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D46" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E46" s="13" t="s">
         <v>199</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>200</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>82</v>
@@ -2585,19 +2148,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B47" s="12">
-        <v>17</v>
+        <v>140</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D47" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E47" s="13" t="s">
         <v>201</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>202</v>
       </c>
       <c r="F47" s="13" t="s">
         <v>102</v>
@@ -2610,17 +2173,17 @@
       <c r="A48" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B48" s="12">
-        <v>18</v>
+      <c r="B48" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D48" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E48" s="12" t="s">
         <v>203</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>204</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>82</v>
@@ -2633,17 +2196,17 @@
       <c r="A49" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="12">
-        <v>19</v>
+      <c r="B49" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D49" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E49" s="13" t="s">
         <v>205</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>206</v>
       </c>
       <c r="F49" s="12" t="s">
         <v>78</v>
@@ -2654,19 +2217,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B50" s="12">
-        <v>20</v>
+        <v>141</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D50" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E50" s="13" t="s">
         <v>207</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>208</v>
       </c>
       <c r="F50" s="13" t="s">
         <v>101</v>
@@ -2679,17 +2242,17 @@
       <c r="A51" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="12">
-        <v>21</v>
+      <c r="B51" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D51" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E51" s="13" t="s">
         <v>209</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>210</v>
       </c>
       <c r="F51" s="13" t="s">
         <v>82</v>
@@ -2720,6 +2283,25 @@
     <hyperlink ref="A47" r:id="rId17" display="e@gmail.com" xr:uid="{24E5F649-4D3B-4574-BFCA-C463472ADE3A}"/>
     <hyperlink ref="A40" r:id="rId18" display="e@gmail.com" xr:uid="{6A205C34-9E54-4767-97DB-C51CBD620646}"/>
     <hyperlink ref="A45" r:id="rId19" display="e@gmail.com" xr:uid="{EAC937D3-2EBB-4C05-88B9-ABDC42FCD2A7}"/>
+    <hyperlink ref="B31" r:id="rId20" display="a@gmail.com" xr:uid="{EAB19170-43BA-4D4F-9332-4F89D76F807A}"/>
+    <hyperlink ref="B34" r:id="rId21" display="f@gmail.com" xr:uid="{EB6D6AAC-34F0-4C79-A8E9-78DF9A5B8425}"/>
+    <hyperlink ref="B33" r:id="rId22" display="c@gmail.com" xr:uid="{5C3346C0-C5AA-42C9-9968-4178F21CFF24}"/>
+    <hyperlink ref="B32" r:id="rId23" display="b@gmail.com" xr:uid="{EF187BD7-B7DF-4809-933B-3228DCE4E6F0}"/>
+    <hyperlink ref="B35" r:id="rId24" display="e@gmail.com" xr:uid="{1E3CE35E-E4C2-4401-A259-19461639BCE0}"/>
+    <hyperlink ref="B36" r:id="rId25" display="a@gmail.com" xr:uid="{7050DA52-748C-4105-9B83-84BD7A66C0D8}"/>
+    <hyperlink ref="B41" r:id="rId26" display="a@gmail.com" xr:uid="{D4D4E4EF-0E24-4BE2-96B8-7363824DCF23}"/>
+    <hyperlink ref="B46" r:id="rId27" display="a@gmail.com" xr:uid="{2898F26E-9244-4586-A47C-C0ADF691C217}"/>
+    <hyperlink ref="B39" r:id="rId28" display="f@gmail.com" xr:uid="{432D20DB-3402-4B76-AA61-162A3ACE2FCF}"/>
+    <hyperlink ref="B44" r:id="rId29" display="f@gmail.com" xr:uid="{DF22C7FA-6CDE-4C05-8C62-69BB83A39F95}"/>
+    <hyperlink ref="B49" r:id="rId30" display="f@gmail.com" xr:uid="{752E6781-06E9-4667-992A-B4B8E10D84F8}"/>
+    <hyperlink ref="B38" r:id="rId31" display="c@gmail.com" xr:uid="{84C8388F-3FBE-468E-8884-20CEB8EB7440}"/>
+    <hyperlink ref="B43" r:id="rId32" display="c@gmail.com" xr:uid="{B71FDC34-B7F9-454C-A404-9D7C7F7B193F}"/>
+    <hyperlink ref="B48" r:id="rId33" display="c@gmail.com" xr:uid="{26D0DD3D-A72E-4E29-92B3-AAA19A595A1E}"/>
+    <hyperlink ref="B37" r:id="rId34" display="b@gmail.com" xr:uid="{93052DCE-A56C-4848-AA6E-06C0E46EA34B}"/>
+    <hyperlink ref="B42" r:id="rId35" display="b@gmail.com" xr:uid="{C182D3A2-0369-445F-9C69-510FFC216F22}"/>
+    <hyperlink ref="B47" r:id="rId36" display="e@gmail.com" xr:uid="{24B86E58-209A-4C26-BCA9-80577EBC4D4F}"/>
+    <hyperlink ref="B40" r:id="rId37" display="e@gmail.com" xr:uid="{8C8BB0AE-FF79-4F92-8F37-4AAE70C76701}"/>
+    <hyperlink ref="B45" r:id="rId38" display="e@gmail.com" xr:uid="{E2CAB3BC-F441-40C0-BEC0-4ECAEBF7402C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2727,10 +2309,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCE681D-66B7-4B70-8FB6-020D9A51E173}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E15"/>
+      <selection activeCell="B2" sqref="B2:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2760,9 +2342,8 @@
       <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14">
-        <f>VLOOKUP(A2,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>1</v>
+      <c r="B2" s="14" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>42</v>
@@ -2778,9 +2359,8 @@
       <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14">
-        <f>VLOOKUP(A3,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>2</v>
+      <c r="B3" s="14" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>41</v>
@@ -2797,9 +2377,8 @@
       <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="14">
-        <f>VLOOKUP(A4,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>3</v>
+      <c r="B4" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>40</v>
@@ -2816,9 +2395,8 @@
       <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="14">
-        <f>VLOOKUP(A5,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>4</v>
+      <c r="B5" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>39</v>
@@ -2835,9 +2413,8 @@
       <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="14">
-        <f>VLOOKUP(A6,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>5</v>
+      <c r="B6" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>43</v>
@@ -2854,9 +2431,8 @@
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="14">
-        <f>VLOOKUP(A7,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>6</v>
+      <c r="B7" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>44</v>
@@ -2872,9 +2448,8 @@
       <c r="A8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="14">
-        <f>VLOOKUP(A8,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>7</v>
+      <c r="B8" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>45</v>
@@ -2890,9 +2465,8 @@
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="14">
-        <f>VLOOKUP(A9,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>8</v>
+      <c r="B9" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>46</v>
@@ -2908,9 +2482,8 @@
       <c r="A10" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="14">
-        <f>VLOOKUP(A10,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>9</v>
+      <c r="B10" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>47</v>
@@ -2926,9 +2499,8 @@
       <c r="A11" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="14">
-        <f>VLOOKUP(A11,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>10</v>
+      <c r="B11" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>48</v>
@@ -2944,9 +2516,8 @@
       <c r="A12" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="14">
-        <f>VLOOKUP(A12,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>11</v>
+      <c r="B12" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>49</v>
@@ -2962,9 +2533,8 @@
       <c r="A13" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="14">
-        <f>VLOOKUP(A13,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>12</v>
+      <c r="B13" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>50</v>
@@ -2980,9 +2550,8 @@
       <c r="A14" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="14">
-        <f>VLOOKUP(A14,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>13</v>
+      <c r="B14" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>51</v>
@@ -2992,24 +2561,6 @@
       </c>
       <c r="E14" s="15">
         <v>43895</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="14">
-        <f>VLOOKUP(A15,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="15">
-        <v>43896</v>
-      </c>
-      <c r="E15" s="15">
-        <v>43896</v>
       </c>
     </row>
   </sheetData>
@@ -3020,10 +2571,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E8"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3055,8 +2606,8 @@
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14">
-        <v>1</v>
+      <c r="B2" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>21</v>
@@ -3072,8 +2623,8 @@
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="14">
-        <v>6</v>
+      <c r="B3" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>22</v>
@@ -3087,94 +2638,27 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="14">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D4" s="15">
-        <v>43896</v>
+        <v>43899</v>
       </c>
       <c r="E4" s="15">
-        <v>43896</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="14">
-        <v>2</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" s="15">
-        <v>43896</v>
-      </c>
-      <c r="E5" s="15">
-        <v>43896</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="14">
-        <v>3</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="D6" s="15">
         <v>43899</v>
-      </c>
-      <c r="E6" s="15">
-        <v>43899</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="14">
-        <f>VLOOKUP(A7,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>11</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="D7" s="15">
-        <v>43899</v>
-      </c>
-      <c r="E7" s="15">
-        <v>43900</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="14">
-        <v>6</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="D8" s="15">
-        <v>43907</v>
-      </c>
-      <c r="E8" s="15">
-        <v>43914</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="a@mail.com" xr:uid="{FFBE8D7A-4F36-46AB-8821-809928F3B807}"/>
     <hyperlink ref="A3" r:id="rId2" display="f@mail.com" xr:uid="{BCFDDFC1-CD43-483B-AF57-67D98952EA36}"/>
+    <hyperlink ref="B2" r:id="rId3" display="a@mail.com" xr:uid="{C25C6478-31DA-4778-86CC-DC6114A163FE}"/>
+    <hyperlink ref="B3" r:id="rId4" display="f@mail.com" xr:uid="{980CB486-383B-4054-B4A0-68946A0B99E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3182,10 +2666,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9E3C4F-9A91-4269-87FF-84A4253640CF}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3216,8 +2700,8 @@
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="14">
-        <v>1</v>
+      <c r="B2" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>37</v>
@@ -3226,15 +2710,15 @@
         <v>43895</v>
       </c>
       <c r="E2" s="15">
-        <v>43896</v>
+        <v>43895</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="14">
-        <v>5</v>
+      <c r="B3" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>38</v>
@@ -3250,8 +2734,8 @@
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14">
-        <v>2</v>
+      <c r="B4" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>37</v>
@@ -3261,24 +2745,6 @@
       </c>
       <c r="E4" s="15">
         <v>43899</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="14">
-        <f>VLOOKUP(A5,[1]Roster!$A$2:$B$51,2,FALSE)</f>
-        <v>11</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="15">
-        <v>43899</v>
-      </c>
-      <c r="E5" s="15">
-        <v>43903</v>
       </c>
     </row>
   </sheetData>
@@ -3286,6 +2752,9 @@
     <hyperlink ref="A2" r:id="rId1" display="b@mail.com" xr:uid="{1BCDC8C4-78E5-4520-987A-A7A37206FD9D}"/>
     <hyperlink ref="A3" r:id="rId2" display="e@mail.com" xr:uid="{556196E9-1FDF-4884-8C20-0C664ECD5F20}"/>
     <hyperlink ref="A4" r:id="rId3" display="b@mail.com" xr:uid="{87E09612-D6DE-48A2-BE0C-C75430DEFFA5}"/>
+    <hyperlink ref="B2" r:id="rId4" display="b@mail.com" xr:uid="{1E46E39C-4AB3-4483-901C-599325B7C246}"/>
+    <hyperlink ref="B3" r:id="rId5" display="e@mail.com" xr:uid="{B30CBBAE-8649-4DD3-A3CF-91BB4C8C1F7E}"/>
+    <hyperlink ref="B4" r:id="rId6" display="b@mail.com" xr:uid="{9011C81C-DB23-4C3D-96B5-09B006763566}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3295,7 +2764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753DE2B1-4FE7-470E-881D-78CA2B270105}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>